<commit_message>
copying data from shared lab folder to git repo
</commit_message>
<xml_diff>
--- a/data/QuestionnairesA.xlsx
+++ b/data/QuestionnairesA.xlsx
@@ -22420,8 +22420,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010077F09E9DF34D434F860A2C878DCE75BD" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="78f79efc5d96fdd80d428a84f71fe178">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56924695-dd61-46fd-8dfa-58e1458a5cd5" xmlns:ns3="c2f508c1-4dad-4dd0-b915-21a5a3be5ef0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86adbb9106985a11906e9c2cc8a6377a" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010077F09E9DF34D434F860A2C878DCE75BD" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4a5d3851d64544f822ba170cf71fd0f5">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56924695-dd61-46fd-8dfa-58e1458a5cd5" xmlns:ns3="c2f508c1-4dad-4dd0-b915-21a5a3be5ef0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e45c0dd3a9809dcc1800ab58abf2b8f" ns2:_="" ns3:_="">
     <xsd:import namespace="56924695-dd61-46fd-8dfa-58e1458a5cd5"/>
     <xsd:import namespace="c2f508c1-4dad-4dd0-b915-21a5a3be5ef0"/>
     <xsd:element name="properties">
@@ -22695,22 +22695,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2B8D712-3693-451E-9942-0285F183CF27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="56924695-dd61-46fd-8dfa-58e1458a5cd5"/>
-    <ds:schemaRef ds:uri="c2f508c1-4dad-4dd0-b915-21a5a3be5ef0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ED75CAD-ADF7-45C5-B2C5-92319367F24F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>